<commit_message>
Replaced openpyxl with pandas for easier testing that files match.
</commit_message>
<xml_diff>
--- a/testfiles/panexport_golden_output.xlsx
+++ b/testfiles/panexport_golden_output.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16828"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jay\Documents\PycharmProjects\pan-os-scripts\testfiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\js201393\Documents\coding\pan-os-scripts\testfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -75,40 +75,40 @@
     <t>Probably important but I'm not sure</t>
   </si>
   <si>
+    <t>Very Important</t>
+  </si>
+  <si>
+    <t>Documentation Group</t>
+  </si>
+  <si>
+    <t>10.11.0.1</t>
+  </si>
+  <si>
+    <t>1.1.1.1</t>
+  </si>
+  <si>
+    <t>2.2.2.2</t>
+  </si>
+  <si>
+    <t>http</t>
+  </si>
+  <si>
+    <t>Internet</t>
+  </si>
+  <si>
+    <t>Syslog</t>
+  </si>
+  <si>
+    <t>tag</t>
+  </si>
+  <si>
+    <t>YOUR IT</t>
+  </si>
+  <si>
+    <t>web-browsing, ssl</t>
+  </si>
+  <si>
     <t>Semi-Important</t>
-  </si>
-  <si>
-    <t>Very Important</t>
-  </si>
-  <si>
-    <t>Documentation Group</t>
-  </si>
-  <si>
-    <t>10.11.0.1</t>
-  </si>
-  <si>
-    <t>1.1.1.1</t>
-  </si>
-  <si>
-    <t>2.2.2.2</t>
-  </si>
-  <si>
-    <t>http</t>
-  </si>
-  <si>
-    <t>Internet</t>
-  </si>
-  <si>
-    <t>Syslog</t>
-  </si>
-  <si>
-    <t>tag</t>
-  </si>
-  <si>
-    <t>YOUR IT</t>
-  </si>
-  <si>
-    <t>web-browsing, ssl</t>
   </si>
 </sst>
 </file>
@@ -239,23 +239,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -291,23 +274,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -486,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,7 +481,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -553,7 +519,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -562,7 +528,7 @@
         <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
@@ -574,10 +540,10 @@
         <v>14</v>
       </c>
       <c r="J2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L2" t="s">
         <v>15</v>
@@ -586,7 +552,7 @@
         <v>16</v>
       </c>
       <c r="N2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -594,19 +560,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G3" t="s">
         <v>14</v>
@@ -615,16 +581,16 @@
         <v>14</v>
       </c>
       <c r="I3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" t="s">
         <v>23</v>
-      </c>
-      <c r="K3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" t="s">
-        <v>24</v>
       </c>
       <c r="M3" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
First cut attempt at re-write excel writing function
</commit_message>
<xml_diff>
--- a/testfiles/panexport_golden_output.xlsx
+++ b/testfiles/panexport_golden_output.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16828"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\js201393\Documents\coding\pan-os-scripts\testfiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jay\Documents\PycharmProjects\pan-os-scripts\testfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,9 +24,6 @@
     <t>Order</t>
   </si>
   <si>
-    <t>@name</t>
-  </si>
-  <si>
     <t>action</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
   </si>
   <si>
     <t>Semi-Important</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -239,6 +239,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -274,6 +291,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -453,7 +487,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,43 +509,43 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -519,40 +553,40 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>15</v>
       </c>
-      <c r="M2" t="s">
-        <v>16</v>
-      </c>
       <c r="N2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -560,40 +594,40 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" t="s">
         <v>22</v>
       </c>
-      <c r="K3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" t="s">
-        <v>23</v>
-      </c>
       <c r="M3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Write excel rewrite (#13)
Rewrite of write_to_excel function to use tablib
</commit_message>
<xml_diff>
--- a/testfiles/panexport_golden_output.xlsx
+++ b/testfiles/panexport_golden_output.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16828"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\js201393\Documents\coding\pan-os-scripts\testfiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jay\Documents\PycharmProjects\pan-os-scripts\testfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,91 +24,91 @@
     <t>Order</t>
   </si>
   <si>
+    <t>action</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>source-user</t>
+  </si>
+  <si>
+    <t>hip-profiles</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>destination</t>
+  </si>
+  <si>
+    <t>application</t>
+  </si>
+  <si>
+    <t>service</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>log-setting</t>
+  </si>
+  <si>
+    <t>allow</t>
+  </si>
+  <si>
+    <t>any</t>
+  </si>
+  <si>
+    <t>application-default</t>
+  </si>
+  <si>
+    <t>This rule is very important, it is at top</t>
+  </si>
+  <si>
+    <t>Probably important but I'm not sure</t>
+  </si>
+  <si>
+    <t>Very Important</t>
+  </si>
+  <si>
+    <t>Documentation Group</t>
+  </si>
+  <si>
+    <t>10.11.0.1</t>
+  </si>
+  <si>
+    <t>1.1.1.1</t>
+  </si>
+  <si>
+    <t>2.2.2.2</t>
+  </si>
+  <si>
+    <t>http</t>
+  </si>
+  <si>
+    <t>Internet</t>
+  </si>
+  <si>
+    <t>Syslog</t>
+  </si>
+  <si>
+    <t>tag</t>
+  </si>
+  <si>
+    <t>YOUR IT</t>
+  </si>
+  <si>
+    <t>web-browsing, ssl</t>
+  </si>
+  <si>
+    <t>Semi-Important</t>
+  </si>
+  <si>
     <t>@name</t>
-  </si>
-  <si>
-    <t>action</t>
-  </si>
-  <si>
-    <t>from</t>
-  </si>
-  <si>
-    <t>source</t>
-  </si>
-  <si>
-    <t>source-user</t>
-  </si>
-  <si>
-    <t>hip-profiles</t>
-  </si>
-  <si>
-    <t>to</t>
-  </si>
-  <si>
-    <t>destination</t>
-  </si>
-  <si>
-    <t>application</t>
-  </si>
-  <si>
-    <t>service</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>log-setting</t>
-  </si>
-  <si>
-    <t>allow</t>
-  </si>
-  <si>
-    <t>any</t>
-  </si>
-  <si>
-    <t>application-default</t>
-  </si>
-  <si>
-    <t>This rule is very important, it is at top</t>
-  </si>
-  <si>
-    <t>Probably important but I'm not sure</t>
-  </si>
-  <si>
-    <t>Very Important</t>
-  </si>
-  <si>
-    <t>Documentation Group</t>
-  </si>
-  <si>
-    <t>10.11.0.1</t>
-  </si>
-  <si>
-    <t>1.1.1.1</t>
-  </si>
-  <si>
-    <t>2.2.2.2</t>
-  </si>
-  <si>
-    <t>http</t>
-  </si>
-  <si>
-    <t>Internet</t>
-  </si>
-  <si>
-    <t>Syslog</t>
-  </si>
-  <si>
-    <t>tag</t>
-  </si>
-  <si>
-    <t>YOUR IT</t>
-  </si>
-  <si>
-    <t>web-browsing, ssl</t>
-  </si>
-  <si>
-    <t>Semi-Important</t>
   </si>
 </sst>
 </file>
@@ -239,6 +239,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -274,6 +291,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -453,7 +487,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,43 +509,43 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -519,40 +553,40 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>15</v>
       </c>
-      <c r="M2" t="s">
-        <v>16</v>
-      </c>
       <c r="N2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -560,40 +594,40 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" t="s">
         <v>22</v>
       </c>
-      <c r="K3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" t="s">
-        <v>23</v>
-      </c>
       <c r="M3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tablib and fixes issue #14 (#15)
* Write excel rewrite (#13)

Rewrite of write_to_excel function to use tablib

* initial regex change to more accurately reflect it is matching ipv4 addresses. Regex is also accurate, avoids capturing 0/101 as defined in issue #14

* ipv6 regex lines, fixes issue #14
</commit_message>
<xml_diff>
--- a/testfiles/panexport_golden_output.xlsx
+++ b/testfiles/panexport_golden_output.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16828"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\js201393\Documents\coding\pan-os-scripts\testfiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jay\Documents\PycharmProjects\pan-os-scripts\testfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,91 +24,91 @@
     <t>Order</t>
   </si>
   <si>
+    <t>action</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>source-user</t>
+  </si>
+  <si>
+    <t>hip-profiles</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>destination</t>
+  </si>
+  <si>
+    <t>application</t>
+  </si>
+  <si>
+    <t>service</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>log-setting</t>
+  </si>
+  <si>
+    <t>allow</t>
+  </si>
+  <si>
+    <t>any</t>
+  </si>
+  <si>
+    <t>application-default</t>
+  </si>
+  <si>
+    <t>This rule is very important, it is at top</t>
+  </si>
+  <si>
+    <t>Probably important but I'm not sure</t>
+  </si>
+  <si>
+    <t>Very Important</t>
+  </si>
+  <si>
+    <t>Documentation Group</t>
+  </si>
+  <si>
+    <t>10.11.0.1</t>
+  </si>
+  <si>
+    <t>1.1.1.1</t>
+  </si>
+  <si>
+    <t>2.2.2.2</t>
+  </si>
+  <si>
+    <t>http</t>
+  </si>
+  <si>
+    <t>Internet</t>
+  </si>
+  <si>
+    <t>Syslog</t>
+  </si>
+  <si>
+    <t>tag</t>
+  </si>
+  <si>
+    <t>YOUR IT</t>
+  </si>
+  <si>
+    <t>web-browsing, ssl</t>
+  </si>
+  <si>
+    <t>Semi-Important</t>
+  </si>
+  <si>
     <t>@name</t>
-  </si>
-  <si>
-    <t>action</t>
-  </si>
-  <si>
-    <t>from</t>
-  </si>
-  <si>
-    <t>source</t>
-  </si>
-  <si>
-    <t>source-user</t>
-  </si>
-  <si>
-    <t>hip-profiles</t>
-  </si>
-  <si>
-    <t>to</t>
-  </si>
-  <si>
-    <t>destination</t>
-  </si>
-  <si>
-    <t>application</t>
-  </si>
-  <si>
-    <t>service</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>log-setting</t>
-  </si>
-  <si>
-    <t>allow</t>
-  </si>
-  <si>
-    <t>any</t>
-  </si>
-  <si>
-    <t>application-default</t>
-  </si>
-  <si>
-    <t>This rule is very important, it is at top</t>
-  </si>
-  <si>
-    <t>Probably important but I'm not sure</t>
-  </si>
-  <si>
-    <t>Very Important</t>
-  </si>
-  <si>
-    <t>Documentation Group</t>
-  </si>
-  <si>
-    <t>10.11.0.1</t>
-  </si>
-  <si>
-    <t>1.1.1.1</t>
-  </si>
-  <si>
-    <t>2.2.2.2</t>
-  </si>
-  <si>
-    <t>http</t>
-  </si>
-  <si>
-    <t>Internet</t>
-  </si>
-  <si>
-    <t>Syslog</t>
-  </si>
-  <si>
-    <t>tag</t>
-  </si>
-  <si>
-    <t>YOUR IT</t>
-  </si>
-  <si>
-    <t>web-browsing, ssl</t>
-  </si>
-  <si>
-    <t>Semi-Important</t>
   </si>
 </sst>
 </file>
@@ -239,6 +239,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -274,6 +291,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -453,7 +487,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,43 +509,43 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -519,40 +553,40 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>15</v>
       </c>
-      <c r="M2" t="s">
-        <v>16</v>
-      </c>
       <c r="N2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -560,40 +594,40 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" t="s">
         <v>22</v>
       </c>
-      <c r="K3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" t="s">
-        <v>23</v>
-      </c>
       <c r="M3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>